<commit_message>
create dataframe from measures in .csv
</commit_message>
<xml_diff>
--- a/Report_Categories.xlsx
+++ b/Report_Categories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eberly\Documents\GitHub\Assess_Industrial-base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A19F1E-A30A-46D5-A73B-6021CCDA5E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1363CA36-DFF9-438F-BBAD-FD724A9B3A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="230" yWindow="2130" windowWidth="14890" windowHeight="13060" xr2:uid="{40FD3958-4C3B-4730-9C22-FF4135E4C237}"/>
+    <workbookView xWindow="3340" yWindow="3340" windowWidth="19200" windowHeight="11260" xr2:uid="{40FD3958-4C3B-4730-9C22-FF4135E4C237}"/>
   </bookViews>
   <sheets>
     <sheet name="Reports_Legend" sheetId="1" r:id="rId1"/>
@@ -1080,8 +1080,8 @@
   </sheetPr>
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1141,7 +1141,7 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">

</xml_diff>